<commit_message>
1.Make Services.java centralized 2.updated core objects
</commit_message>
<xml_diff>
--- a/core/src/main/resources/Sanity.xlsx
+++ b/core/src/main/resources/Sanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Master\Automation_Project\core\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7251F596-FDC0-4062-8D4D-06C47CB0BBFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C56B5E-0A50-428F-8F86-58FD0016D0AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="49">
   <si>
     <t>TCID</t>
   </si>
@@ -157,6 +157,27 @@
   </si>
   <si>
     <t>ServiceTests//DummySheet.xlsx</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>JDServices</t>
+  </si>
+  <si>
+    <t>CRUD</t>
+  </si>
+  <si>
+    <t>JDservices.CRUD</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>LocationsServices.CRUD</t>
+  </si>
+  <si>
+    <t>LocationsServices</t>
   </si>
 </sst>
 </file>
@@ -508,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -734,6 +755,52 @@
         <v>8</v>
       </c>
     </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>

</xml_diff>